<commit_message>
can draw all GameEntity
</commit_message>
<xml_diff>
--- a/docs/数值策划.xlsx
+++ b/docs/数值策划.xlsx
@@ -108,9 +108,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
@@ -123,14 +123,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -150,9 +166,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -160,29 +191,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -197,8 +213,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -208,30 +239,6 @@
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -251,16 +258,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -293,55 +293,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -359,7 +347,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -371,25 +413,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -401,37 +461,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -443,37 +473,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -515,21 +515,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -545,11 +530,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -580,15 +571,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -612,6 +594,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -620,10 +620,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -632,133 +632,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1121,7 +1121,7 @@
   <dimension ref="A1:AF91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.625" defaultRowHeight="13.5"/>
@@ -1191,6 +1191,9 @@
       <c r="F2">
         <v>10</v>
       </c>
+      <c r="G2">
+        <v>100</v>
+      </c>
       <c r="H2">
         <v>3000</v>
       </c>
@@ -1465,7 +1468,10 @@
         <v>5</v>
       </c>
       <c r="S9">
-        <v>50</v>
+        <v>25</v>
+      </c>
+      <c r="T9">
+        <v>5</v>
       </c>
       <c r="Z9" s="2">
         <f>S9*$B$2+T9*$C$2+V9*$E$2+W9*$F$2+X9*$G$2+Y9*$H$2</f>
@@ -1480,15 +1486,15 @@
         <v>2</v>
       </c>
       <c r="AD9">
-        <f t="shared" ref="AD9:AD14" si="4">AD8+AF8</f>
+        <f t="shared" ref="AD9:AD19" si="4">AD8+AF8</f>
         <v>33</v>
       </c>
       <c r="AE9">
-        <f t="shared" ref="AE9:AE14" si="5">AD9</f>
+        <f t="shared" ref="AE9:AE19" si="5">AD9</f>
         <v>33</v>
       </c>
       <c r="AF9">
-        <f t="shared" ref="AF9:AF14" si="6">AE9*$AF$5</f>
+        <f t="shared" ref="AF9:AF19" si="6">AE9*$AF$5</f>
         <v>3.3</v>
       </c>
     </row>
@@ -1605,6 +1611,9 @@
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
+      <c r="S12">
+        <v>50</v>
+      </c>
       <c r="T12">
         <v>5</v>
       </c>
@@ -1613,7 +1622,7 @@
       </c>
       <c r="Z12" s="2">
         <f>S12*$B$2+T12*$C$2+V12*$E$2+W12*$F$2+X12*$G$2+Y12*$H$2</f>
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="AA12" s="2"/>
       <c r="AB12">
@@ -1640,12 +1649,9 @@
       <c r="A13" t="s">
         <v>25</v>
       </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
       <c r="I13" s="1">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M13">
         <v>1</v>
@@ -1653,17 +1659,16 @@
       <c r="N13">
         <v>3</v>
       </c>
-      <c r="O13"/>
       <c r="Q13" s="2">
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="R13" s="3">
         <f t="shared" si="3"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="S13">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="T13">
         <v>15</v>
@@ -1671,9 +1676,12 @@
       <c r="V13">
         <v>5</v>
       </c>
+      <c r="W13">
+        <v>5</v>
+      </c>
       <c r="Z13" s="2">
         <f>S13*$B$2+T13*$C$2+V13*$E$2+W13*$F$2+X13*$G$2+Y13*$H$2</f>
-        <v>200</v>
+        <v>350</v>
       </c>
       <c r="AA13" s="2"/>
       <c r="AB13">
@@ -1700,12 +1708,9 @@
       <c r="A14" t="s">
         <v>26</v>
       </c>
-      <c r="C14">
-        <v>10</v>
-      </c>
       <c r="I14" s="1">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="M14">
         <v>3</v>
@@ -1716,18 +1721,32 @@
       <c r="O14">
         <v>1</v>
       </c>
-      <c r="P14"/>
       <c r="Q14" s="2">
         <f t="shared" si="2"/>
-        <v>65</v>
+        <v>165</v>
       </c>
       <c r="R14" s="3">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>165</v>
+      </c>
+      <c r="S14">
+        <v>500</v>
+      </c>
+      <c r="T14">
+        <v>30</v>
+      </c>
+      <c r="U14">
+        <v>5</v>
+      </c>
+      <c r="V14">
+        <v>10</v>
+      </c>
+      <c r="W14">
+        <v>10</v>
       </c>
       <c r="Z14" s="2">
         <f t="shared" ref="Z11:Z33" si="7">S14*$B$2+T14*$C$2+V14*$E$2+W14*$F$2+X14*$G$2+Y14*$H$2</f>
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="AA14" s="2"/>
       <c r="AB14">
@@ -1754,20 +1773,9 @@
       <c r="A15" t="s">
         <v>27</v>
       </c>
-      <c r="C15">
-        <v>30</v>
-      </c>
-      <c r="E15">
-        <v>5</v>
-      </c>
-      <c r="F15">
-        <v>5</v>
-      </c>
-      <c r="G15"/>
-      <c r="H15"/>
       <c r="I15" s="1">
         <f t="shared" si="1"/>
-        <v>225</v>
+        <v>0</v>
       </c>
       <c r="P15">
         <v>1</v>
@@ -1778,13 +1786,13 @@
       </c>
       <c r="R15" s="3">
         <f t="shared" si="3"/>
-        <v>2775</v>
+        <v>3000</v>
       </c>
       <c r="S15">
         <v>5000</v>
       </c>
       <c r="T15">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="U15">
         <v>50</v>
@@ -1800,7 +1808,7 @@
       </c>
       <c r="Z15" s="2">
         <f t="shared" si="7"/>
-        <v>8500</v>
+        <v>7000</v>
       </c>
       <c r="AA15" s="2"/>
       <c r="AB15">
@@ -1811,15 +1819,15 @@
         <v>8</v>
       </c>
       <c r="AD15">
-        <f>AD14+AF14</f>
+        <f t="shared" si="4"/>
         <v>58.461513</v>
       </c>
       <c r="AE15">
-        <f>AD15</f>
+        <f t="shared" si="5"/>
         <v>58.461513</v>
       </c>
       <c r="AF15">
-        <f>AE15*$AF$5</f>
+        <f t="shared" si="6"/>
         <v>5.8461513</v>
       </c>
     </row>
@@ -1849,15 +1857,15 @@
         <v>9</v>
       </c>
       <c r="AD16">
-        <f>AD15+AF15</f>
+        <f t="shared" si="4"/>
         <v>64.3076643</v>
       </c>
       <c r="AE16">
-        <f>AD16</f>
+        <f t="shared" si="5"/>
         <v>64.3076643</v>
       </c>
       <c r="AF16">
-        <f>AE16*$AF$5</f>
+        <f t="shared" si="6"/>
         <v>6.43076643</v>
       </c>
     </row>
@@ -1887,15 +1895,15 @@
         <v>10</v>
       </c>
       <c r="AD17">
-        <f>AD16+AF16</f>
+        <f t="shared" si="4"/>
         <v>70.73843073</v>
       </c>
       <c r="AE17">
-        <f>AD17</f>
+        <f t="shared" si="5"/>
         <v>70.73843073</v>
       </c>
       <c r="AF17">
-        <f>AE17*$AF$5</f>
+        <f t="shared" si="6"/>
         <v>7.073843073</v>
       </c>
     </row>
@@ -1904,11 +1912,11 @@
         <v>28</v>
       </c>
       <c r="H18">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I18" s="1">
         <f t="shared" si="1"/>
-        <v>3000000</v>
+        <v>1500000</v>
       </c>
       <c r="Q18" s="2">
         <f t="shared" si="2"/>
@@ -1916,7 +1924,7 @@
       </c>
       <c r="R18" s="3">
         <f t="shared" si="3"/>
-        <v>-3000000</v>
+        <v>-1500000</v>
       </c>
       <c r="Z18" s="2">
         <f t="shared" si="7"/>
@@ -1931,15 +1939,15 @@
         <v>11</v>
       </c>
       <c r="AD18">
-        <f>AD17+AF17</f>
+        <f t="shared" si="4"/>
         <v>77.812273803</v>
       </c>
       <c r="AE18">
-        <f>AD18</f>
+        <f t="shared" si="5"/>
         <v>77.812273803</v>
       </c>
       <c r="AF18">
-        <f>AE18*$AF$5</f>
+        <f t="shared" si="6"/>
         <v>7.7812273803</v>
       </c>
     </row>
@@ -1969,15 +1977,15 @@
         <v>12</v>
       </c>
       <c r="AD19">
-        <f>AD18+AF18</f>
+        <f t="shared" si="4"/>
         <v>85.5935011833</v>
       </c>
       <c r="AE19">
-        <f>AD19</f>
+        <f t="shared" si="5"/>
         <v>85.5935011833</v>
       </c>
       <c r="AF19">
-        <f>AE19*$AF$5</f>
+        <f t="shared" si="6"/>
         <v>8.55935011833</v>
       </c>
     </row>

</xml_diff>